<commit_message>
Add lifetime calculation to Uncertainty_Propagation.py
</commit_message>
<xml_diff>
--- a/Calc_Width_Lifetime.xlsx
+++ b/Calc_Width_Lifetime.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Si24\root_scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F09EA32-52D0-4A76-ABD9-A6F9FA2AC163}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{483A74E2-4D99-4AE8-AB2F-7234F7D398BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8004" yWindow="-24" windowWidth="15144" windowHeight="12000" xr2:uid="{54B87DC3-80D2-408F-9ECA-DC6AAEA4FCE2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{54B87DC3-80D2-408F-9ECA-DC6AAEA4FCE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,9 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -1934,7 +1937,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2029,7 +2032,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="6">
-        <v>72000</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>3</v>
@@ -2052,7 +2055,7 @@
       </c>
       <c r="B7" s="3">
         <f>B6/$B$2</f>
-        <v>7.1999999999999995E-2</v>
+        <v>5.0000000000000001E-9</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>8</v>
@@ -2075,7 +2078,7 @@
       </c>
       <c r="B8" s="2">
         <f>B4/$B$6</f>
-        <v>9.1418327347222223E-21</v>
+        <v>1.3164239138000002E-13</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>4</v>
@@ -2098,7 +2101,7 @@
       </c>
       <c r="B9" s="9">
         <f>B8*$B$3</f>
-        <v>9.1418327347222216E-6</v>
+        <v>131.64239138000002</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>9</v>
@@ -2121,7 +2124,7 @@
       </c>
       <c r="B10" s="8">
         <f>B9*LN(2)</f>
-        <v>6.3366355852233222E-6</v>
+        <v>91.247552427215865</v>
       </c>
       <c r="C10" s="1" t="str">
         <f>C9</f>

</xml_diff>